<commit_message>
Iterating through all columns
</commit_message>
<xml_diff>
--- a/Projecto/Data_for_Sarah.xlsx
+++ b/Projecto/Data_for_Sarah.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="15320" activeTab="1"/>
+    <workbookView xWindow="2000" yWindow="-80" windowWidth="21600" windowHeight="15320"/>
   </bookViews>
   <sheets>
     <sheet name="Signal" sheetId="1" r:id="rId1"/>
@@ -333,12 +333,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="8">
     <font>
       <sz val="12"/>
@@ -1096,9 +1090,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AL148"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A15" sqref="A15:AK148"/>
+    <sheetView tabSelected="1" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -3075,7 +3069,9 @@
         <f t="shared" si="0"/>
         <v>0.74759945130315497</v>
       </c>
-      <c r="C24" s="30"/>
+      <c r="C24" s="30">
+        <v>17</v>
+      </c>
       <c r="D24" s="30">
         <v>27</v>
       </c>
@@ -14376,7 +14372,6 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -14389,7 +14384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="F1" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:AK1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
One function iterating over 7 analytes
</commit_message>
<xml_diff>
--- a/Projecto/Data_for_Sarah.xlsx
+++ b/Projecto/Data_for_Sarah.xlsx
@@ -333,6 +333,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <sz val="12"/>
@@ -1090,9 +1096,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AL148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -4096,8 +4102,8 @@
       <c r="J37" s="23">
         <v>63773</v>
       </c>
-      <c r="K37" s="23" t="e">
-        <v>#DIV/0!</v>
+      <c r="K37" s="23">
+        <v>63773</v>
       </c>
       <c r="L37" s="23">
         <v>62385.5</v>
@@ -4870,6 +4876,9 @@
       <c r="B44" s="41">
         <f t="shared" si="1"/>
         <v>0.69913122999542743</v>
+      </c>
+      <c r="C44" s="31">
+        <v>11</v>
       </c>
       <c r="D44" s="31">
         <v>24.5</v>
@@ -14370,8 +14379,10 @@
       <c r="AK148" s="52"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>